<commit_message>
Verification corrections: Add missing Ableton Push 3, mark APC40 MkII as Verified and currently available
</commit_message>
<xml_diff>
--- a/ableton_control_surfaces_catalog.xlsx
+++ b/ableton_control_surfaces_catalog.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D181"/>
+  <dimension ref="A1:D182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -582,90 +583,91 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Push 3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.ableton.com/en/shop/push/</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Controller: $999 USD | Standalone: $1,999 USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Move</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="inlineStr">
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>https://www.ableton.com/en/move/</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>$499 USD / €499 EUR</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Akai Professional</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="4" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="inlineStr">
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="4" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C10" s="5" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>ADVANCE</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>https://www.akaipro.com/</t>
-        </is>
-      </c>
-      <c r="D11" s="8" t="inlineStr">
-        <is>
-          <t>MSRP varies | Not available</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>Akai Force MPC</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>ADVANCE</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C12" s="8" t="inlineStr">
@@ -675,19 +677,19 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>$1,499 USD</t>
+          <t>MSRP varies | Not available</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>APC20</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Akai Force MPC</t>
+        </is>
+      </c>
+      <c r="B13" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C13" s="8" t="inlineStr">
@@ -697,14 +699,14 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Used market only</t>
+          <t>$1,499 USD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>APC40 (Original)</t>
+          <t>APC20</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
@@ -714,19 +716,19 @@
       </c>
       <c r="C14" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc40.html</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP unknown | Used market only</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>APC40 MkII</t>
+          <t>APC40 (Original)</t>
         </is>
       </c>
       <c r="B15" s="7" t="inlineStr">
@@ -736,129 +738,129 @@
       </c>
       <c r="C15" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc40-mkii</t>
+          <t>https://www.akaipro.com/apc40.html</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>$230+ (limited stock)</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
-          <t>APC64</t>
-        </is>
-      </c>
-      <c r="B16" s="9" t="inlineStr">
+          <t>APC40 MkII</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
         <is>
           <t>Verified</t>
         </is>
       </c>
       <c r="C16" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc64.html</t>
+          <t>https://www.akaipro.com/apc40-mkii</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $399 | Current: $189-399</t>
+          <t>Available at authorized retailers</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>APC Key 25</t>
-        </is>
-      </c>
-      <c r="B17" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>APC64</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C17" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc-key-25</t>
+          <t>https://www.akaipro.com/apc64.html</t>
         </is>
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP: $399 | Current: $189-399</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>APC Key 25 mk2</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>APC Key 25</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C18" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc-key-25-mkii.html</t>
+          <t>https://www.akaipro.com/apc-key-25</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $99 USD</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>APC mini</t>
-        </is>
-      </c>
-      <c r="B19" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>APC Key 25 mk2</t>
+        </is>
+      </c>
+      <c r="B19" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C19" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc-mini</t>
+          <t>https://www.akaipro.com/apc-key-25-mkii.html</t>
         </is>
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $99 | Superseded</t>
+          <t>MSRP: $99 USD</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>APC mini mk2</t>
-        </is>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>APC mini</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C20" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/apc-mini-mk2.html</t>
+          <t>https://www.akaipro.com/apc-mini</t>
         </is>
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $99 USD</t>
+          <t>MSRP: $99 | Superseded</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
         <is>
-          <t>LPD8</t>
+          <t>APC mini mk2</t>
         </is>
       </c>
       <c r="B21" s="9" t="inlineStr">
@@ -868,19 +870,19 @@
       </c>
       <c r="C21" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/apc-mini-mk2.html</t>
         </is>
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>Limited availability</t>
+          <t>MSRP: $99 USD</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>MIDI Mix</t>
+          <t>LPD8</t>
         </is>
       </c>
       <c r="B22" s="9" t="inlineStr">
@@ -895,19 +897,19 @@
       </c>
       <c r="D22" s="8" t="inlineStr">
         <is>
-          <t>Pricing varies</t>
+          <t>Limited availability</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>MPD18</t>
-        </is>
-      </c>
-      <c r="B23" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>MIDI Mix</t>
+        </is>
+      </c>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C23" s="8" t="inlineStr">
@@ -917,14 +919,14 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>Pricing varies</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>MPD24</t>
+          <t>MPD18</t>
         </is>
       </c>
       <c r="B24" s="7" t="inlineStr">
@@ -946,7 +948,7 @@
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>MPD32</t>
+          <t>MPD24</t>
         </is>
       </c>
       <c r="B25" s="7" t="inlineStr">
@@ -968,29 +970,29 @@
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>MPD218</t>
-        </is>
-      </c>
-      <c r="B26" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>MPD32</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C26" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpd218</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $199 USD</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>MPD226</t>
+          <t>MPD218</t>
         </is>
       </c>
       <c r="B27" s="9" t="inlineStr">
@@ -1000,19 +1002,19 @@
       </c>
       <c r="C27" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/mpd218</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $299 USD</t>
+          <t>MSRP: $199 USD</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>MPD232</t>
+          <t>MPD226</t>
         </is>
       </c>
       <c r="B28" s="9" t="inlineStr">
@@ -1027,36 +1029,36 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $399 USD</t>
+          <t>MSRP: $299 USD</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>MPK25</t>
-        </is>
-      </c>
-      <c r="B29" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>MPD232</t>
+        </is>
+      </c>
+      <c r="B29" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C29" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk25</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>MSRP: $399 USD</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>MPK49</t>
+          <t>MPK25</t>
         </is>
       </c>
       <c r="B30" s="7" t="inlineStr">
@@ -1066,7 +1068,7 @@
       </c>
       <c r="C30" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/mpk25</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
@@ -1078,7 +1080,7 @@
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>MPK61</t>
+          <t>MPK49</t>
         </is>
       </c>
       <c r="B31" s="7" t="inlineStr">
@@ -1088,7 +1090,7 @@
       </c>
       <c r="C31" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk61.html</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
@@ -1100,7 +1102,7 @@
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>MPK88</t>
+          <t>MPK61</t>
         </is>
       </c>
       <c r="B32" s="7" t="inlineStr">
@@ -1110,7 +1112,7 @@
       </c>
       <c r="C32" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/mpk61.html</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
@@ -1122,29 +1124,29 @@
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>MPK225</t>
-        </is>
-      </c>
-      <c r="B33" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>MPK88</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C33" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk225</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $249.99 | Current: $85+</t>
+          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>MPK249</t>
+          <t>MPK225</t>
         </is>
       </c>
       <c r="B34" s="9" t="inlineStr">
@@ -1154,19 +1156,19 @@
       </c>
       <c r="C34" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/mpk225</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $399.99 | Varies</t>
+          <t>MSRP: $249.99 | Current: $85+</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
         <is>
-          <t>MPK261</t>
+          <t>MPK249</t>
         </is>
       </c>
       <c r="B35" s="9" t="inlineStr">
@@ -1176,46 +1178,46 @@
       </c>
       <c r="C35" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk261</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D35" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $499.99</t>
+          <t>MSRP: $399.99 | Varies</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>MPK mini mk1</t>
-        </is>
-      </c>
-      <c r="B36" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>MPK261</t>
+        </is>
+      </c>
+      <c r="B36" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C36" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/</t>
+          <t>https://www.akaipro.com/mpk261</t>
         </is>
       </c>
       <c r="D36" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP: $499.99</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>MPK mini mkII</t>
-        </is>
-      </c>
-      <c r="B37" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>MPK mini mk1</t>
+        </is>
+      </c>
+      <c r="B37" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C37" s="8" t="inlineStr">
@@ -1225,14 +1227,14 @@
       </c>
       <c r="D37" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>MPK mini mkIII</t>
+          <t>MPK mini mkII</t>
         </is>
       </c>
       <c r="B38" s="9" t="inlineStr">
@@ -1242,19 +1244,19 @@
       </c>
       <c r="C38" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk-mini-mk3</t>
+          <t>https://www.akaipro.com/</t>
         </is>
       </c>
       <c r="D38" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $119</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
         <is>
-          <t>MPK mini Plus</t>
+          <t>MPK mini mkIII</t>
         </is>
       </c>
       <c r="B39" s="9" t="inlineStr">
@@ -1264,95 +1266,96 @@
       </c>
       <c r="C39" s="8" t="inlineStr">
         <is>
-          <t>https://www.akaipro.com/mpk-mini-plus.html</t>
+          <t>https://www.akaipro.com/mpk-mini-mk3</t>
         </is>
       </c>
       <c r="D39" s="8" t="inlineStr">
         <is>
-          <t>Available at retailers</t>
+          <t>MSRP: $119</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
         <is>
+          <t>MPK mini Plus</t>
+        </is>
+      </c>
+      <c r="B40" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C40" s="8" t="inlineStr">
+        <is>
+          <t>https://www.akaipro.com/mpk-mini-plus.html</t>
+        </is>
+      </c>
+      <c r="D40" s="8" t="inlineStr">
+        <is>
+          <t>Available at retailers</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
           <t>MPK mini mk4</t>
         </is>
       </c>
-      <c r="B40" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C40" s="8" t="inlineStr">
+      <c r="B41" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C41" s="8" t="inlineStr">
         <is>
           <t>https://www.akaipro.com/mpk-mini-4.html</t>
         </is>
       </c>
-      <c r="D40" s="8" t="inlineStr">
+      <c r="D41" s="8" t="inlineStr">
         <is>
           <t>2025 release</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr">
+    <row r="42"/>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>Alesis</t>
         </is>
       </c>
-      <c r="B42" s="3" t="n"/>
-      <c r="C42" s="3" t="n"/>
-      <c r="D42" s="4" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="5" t="inlineStr">
+      <c r="B43" s="3" t="n"/>
+      <c r="C43" s="3" t="n"/>
+      <c r="D43" s="4" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B43" s="5" t="inlineStr">
+      <c r="B44" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C43" s="5" t="inlineStr">
+      <c r="C44" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D43" s="5" t="inlineStr">
+      <c r="D44" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="6" t="inlineStr">
-        <is>
-          <t>Alesis V</t>
-        </is>
-      </c>
-      <c r="B44" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C44" s="8" t="inlineStr">
-        <is>
-          <t>https://www.alesis.com/</t>
-        </is>
-      </c>
-      <c r="D44" s="8" t="inlineStr">
-        <is>
-          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>Alesis VI</t>
+          <t>Alesis V</t>
         </is>
       </c>
       <c r="B45" s="7" t="inlineStr">
@@ -1374,7 +1377,7 @@
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>Alesis VX</t>
+          <t>Alesis VI</t>
         </is>
       </c>
       <c r="B46" s="7" t="inlineStr">
@@ -1396,7 +1399,7 @@
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>MasterControl</t>
+          <t>Alesis VX</t>
         </is>
       </c>
       <c r="B47" s="7" t="inlineStr">
@@ -1406,19 +1409,19 @@
       </c>
       <c r="C47" s="8" t="inlineStr">
         <is>
-          <t>https://www.alesis.com/products/view/mastercontrol</t>
+          <t>https://www.alesis.com/</t>
         </is>
       </c>
       <c r="D47" s="8" t="inlineStr">
         <is>
-          <t>MSRP: ~$200 | Discontinued</t>
+          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
         <is>
-          <t>Photon 25</t>
+          <t>MasterControl</t>
         </is>
       </c>
       <c r="B48" s="7" t="inlineStr">
@@ -1428,19 +1431,19 @@
       </c>
       <c r="C48" s="8" t="inlineStr">
         <is>
-          <t>https://www.alesis.com/</t>
+          <t>https://www.alesis.com/products/view/mastercontrol</t>
         </is>
       </c>
       <c r="D48" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown</t>
+          <t>MSRP: ~$200 | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
         <is>
-          <t>Photon X25</t>
+          <t>Photon 25</t>
         </is>
       </c>
       <c r="B49" s="7" t="inlineStr">
@@ -1462,83 +1465,84 @@
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
         <is>
+          <t>Photon X25</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C50" s="8" t="inlineStr">
+        <is>
+          <t>https://www.alesis.com/</t>
+        </is>
+      </c>
+      <c r="D50" s="8" t="inlineStr">
+        <is>
+          <t>MSRP unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
           <t>VCM600</t>
         </is>
       </c>
-      <c r="B50" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C50" s="8" t="inlineStr">
+      <c r="B51" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C51" s="8" t="inlineStr">
         <is>
           <t>https://www.alesis.com/</t>
         </is>
       </c>
-      <c r="D50" s="8" t="inlineStr">
+      <c r="D51" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="inlineStr">
+    <row r="52"/>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
         <is>
           <t>Arturia</t>
         </is>
       </c>
-      <c r="B52" s="3" t="n"/>
-      <c r="C52" s="3" t="n"/>
-      <c r="D52" s="4" t="n"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="5" t="inlineStr">
+      <c r="B53" s="3" t="n"/>
+      <c r="C53" s="3" t="n"/>
+      <c r="D53" s="4" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B53" s="5" t="inlineStr">
+      <c r="B54" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C53" s="5" t="inlineStr">
+      <c r="C54" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D53" s="5" t="inlineStr">
+      <c r="D54" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="6" t="inlineStr">
-        <is>
-          <t>BeatStep</t>
-        </is>
-      </c>
-      <c r="B54" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C54" s="8" t="inlineStr">
-        <is>
-          <t>https://www.arturia.com/products/hybrid-synths/beatstep/overview</t>
-        </is>
-      </c>
-      <c r="D54" s="8" t="inlineStr">
-        <is>
-          <t>$99+</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
         <is>
-          <t>BeatStep Pro</t>
+          <t>BeatStep</t>
         </is>
       </c>
       <c r="B55" s="9" t="inlineStr">
@@ -1548,63 +1552,63 @@
       </c>
       <c r="C55" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/store/beatstep-pro</t>
+          <t>https://www.arturia.com/products/hybrid-synths/beatstep/overview</t>
         </is>
       </c>
       <c r="D55" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $299 | Current: $250-299</t>
+          <t>$99+</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
         <is>
-          <t>KeyLab 88 (Original)</t>
-        </is>
-      </c>
-      <c r="B56" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>BeatStep Pro</t>
+        </is>
+      </c>
+      <c r="B56" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C56" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/</t>
+          <t>https://www.arturia.com/store/beatstep-pro</t>
         </is>
       </c>
       <c r="D56" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP: $299 | Current: $250-299</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>KeyLab 88 MkII</t>
-        </is>
-      </c>
-      <c r="B57" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>KeyLab 88 (Original)</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C57" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/products/hybrid-synths/keylab-88-mkii/overview</t>
+          <t>https://www.arturia.com/</t>
         </is>
       </c>
       <c r="D57" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>KeyLab 88 mk3</t>
+          <t>KeyLab 88 MkII</t>
         </is>
       </c>
       <c r="B58" s="9" t="inlineStr">
@@ -1614,7 +1618,7 @@
       </c>
       <c r="C58" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/products/hybrid-synths/keylab-88-mk3/overview</t>
+          <t>https://www.arturia.com/products/hybrid-synths/keylab-88-mkii/overview</t>
         </is>
       </c>
       <c r="D58" s="8" t="inlineStr">
@@ -1626,51 +1630,51 @@
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
         <is>
-          <t>KeyLab Essential</t>
-        </is>
-      </c>
-      <c r="B59" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>KeyLab 88 mk3</t>
+        </is>
+      </c>
+      <c r="B59" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C59" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/</t>
+          <t>https://www.arturia.com/products/hybrid-synths/keylab-88-mk3/overview</t>
         </is>
       </c>
       <c r="D59" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
         <is>
-          <t>KeyLab Essential mk3 (49/61/88)</t>
-        </is>
-      </c>
-      <c r="B60" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>KeyLab Essential</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C60" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/products/hybrid-synths/keylab-essential-mk3/overview</t>
+          <t>https://www.arturia.com/</t>
         </is>
       </c>
       <c r="D60" s="8" t="inlineStr">
         <is>
-          <t>$219-269</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
         <is>
-          <t>KeyLab mk3 (49/61)</t>
+          <t>KeyLab Essential mk3 (49/61/88)</t>
         </is>
       </c>
       <c r="B61" s="9" t="inlineStr">
@@ -1680,19 +1684,19 @@
       </c>
       <c r="C61" s="8" t="inlineStr">
         <is>
-          <t>https://www.arturia.com/</t>
+          <t>https://www.arturia.com/products/hybrid-synths/keylab-essential-mk3/overview</t>
         </is>
       </c>
       <c r="D61" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>$219-269</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="6" t="inlineStr">
         <is>
-          <t>KeyLab mkII (49/61)</t>
+          <t>KeyLab mk3 (49/61)</t>
         </is>
       </c>
       <c r="B62" s="9" t="inlineStr">
@@ -1714,12 +1718,12 @@
     <row r="63">
       <c r="A63" s="6" t="inlineStr">
         <is>
-          <t>MiniLab (1st Gen)</t>
-        </is>
-      </c>
-      <c r="B63" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>KeyLab mkII (49/61)</t>
+        </is>
+      </c>
+      <c r="B63" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C63" s="8" t="inlineStr">
@@ -1729,19 +1733,19 @@
       </c>
       <c r="D63" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
         <is>
-          <t>MiniLab mkII</t>
-        </is>
-      </c>
-      <c r="B64" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>MiniLab (1st Gen)</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C64" s="8" t="inlineStr">
@@ -1751,448 +1755,454 @@
       </c>
       <c r="D64" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="6" t="inlineStr">
         <is>
+          <t>MiniLab mkII</t>
+        </is>
+      </c>
+      <c r="B65" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C65" s="8" t="inlineStr">
+        <is>
+          <t>https://www.arturia.com/</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="inlineStr">
+        <is>
           <t>MiniLab 3</t>
         </is>
       </c>
-      <c r="B65" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C65" s="8" t="inlineStr">
+      <c r="B66" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C66" s="8" t="inlineStr">
         <is>
           <t>https://www.arturia.com/products/hybrid-synths/minilab-3/overview</t>
         </is>
       </c>
-      <c r="D65" s="8" t="inlineStr">
+      <c r="D66" s="8" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="inlineStr">
+    <row r="67"/>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
         <is>
           <t>Behringer</t>
         </is>
       </c>
-      <c r="B67" s="3" t="n"/>
-      <c r="C67" s="3" t="n"/>
-      <c r="D67" s="4" t="n"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="5" t="inlineStr">
+      <c r="B68" s="3" t="n"/>
+      <c r="C68" s="3" t="n"/>
+      <c r="D68" s="4" t="n"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B68" s="5" t="inlineStr">
+      <c r="B69" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C68" s="5" t="inlineStr">
+      <c r="C69" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D68" s="5" t="inlineStr">
+      <c r="D69" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="6" t="inlineStr">
-        <is>
-          <t>BCF2000</t>
-        </is>
-      </c>
-      <c r="B69" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C69" s="8" t="inlineStr">
-        <is>
-          <t>https://www.behringer.com/behringer/product?modelCode=P0246</t>
-        </is>
-      </c>
-      <c r="D69" s="8" t="inlineStr">
-        <is>
-          <t>MSRP unknown | Used only</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="6" t="inlineStr">
         <is>
+          <t>BCF2000</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C70" s="8" t="inlineStr">
+        <is>
+          <t>https://www.behringer.com/behringer/product?modelCode=P0246</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>MSRP unknown | Used only</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
           <t>BCR2000</t>
         </is>
       </c>
-      <c r="B70" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C70" s="8" t="inlineStr">
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C71" s="8" t="inlineStr">
         <is>
           <t>https://www.behringer.com/</t>
         </is>
       </c>
-      <c r="D70" s="8" t="inlineStr">
+      <c r="D71" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Being replaced</t>
         </is>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="inlineStr">
+    <row r="72"/>
+    <row r="73">
+      <c r="A73" s="2" t="inlineStr">
         <is>
           <t>Blackstar</t>
         </is>
       </c>
-      <c r="B72" s="3" t="n"/>
-      <c r="C72" s="3" t="n"/>
-      <c r="D72" s="4" t="n"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="5" t="inlineStr">
+      <c r="B73" s="3" t="n"/>
+      <c r="C73" s="3" t="n"/>
+      <c r="D73" s="4" t="n"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B73" s="5" t="inlineStr">
+      <c r="B74" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C73" s="5" t="inlineStr">
+      <c r="C74" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D73" s="5" t="inlineStr">
+      <c r="D74" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
         </is>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="6" t="inlineStr">
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
         <is>
           <t>Blackstar Live Logic</t>
         </is>
       </c>
-      <c r="B74" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C74" s="8" t="inlineStr">
+      <c r="B75" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C75" s="8" t="inlineStr">
         <is>
           <t>https://blackstaramps.com/live-logic/</t>
         </is>
       </c>
-      <c r="D74" s="8" t="inlineStr">
+      <c r="D75" s="8" t="inlineStr">
         <is>
           <t>$125+</t>
         </is>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="inlineStr">
+    <row r="76"/>
+    <row r="77">
+      <c r="A77" s="2" t="inlineStr">
         <is>
           <t>Faderfox</t>
         </is>
       </c>
-      <c r="B76" s="3" t="n"/>
-      <c r="C76" s="3" t="n"/>
-      <c r="D76" s="4" t="n"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="5" t="inlineStr">
+      <c r="B77" s="3" t="n"/>
+      <c r="C77" s="3" t="n"/>
+      <c r="D77" s="4" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B77" s="5" t="inlineStr">
+      <c r="B78" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C77" s="5" t="inlineStr">
+      <c r="C78" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D77" s="5" t="inlineStr">
+      <c r="D78" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="6" t="inlineStr">
-        <is>
-          <t>LV1 LX1</t>
-        </is>
-      </c>
-      <c r="B78" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C78" s="8" t="inlineStr">
-        <is>
-          <t>http://faderfox.de/lv1-lx1-dj1.html</t>
-        </is>
-      </c>
-      <c r="D78" s="8" t="inlineStr">
-        <is>
-          <t>Original: ~€200 | Used: $100-175</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="6" t="inlineStr">
         <is>
+          <t>LV1 LX1</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C79" s="8" t="inlineStr">
+        <is>
+          <t>http://faderfox.de/lv1-lx1-dj1.html</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>Original: ~€200 | Used: $100-175</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="6" t="inlineStr">
+        <is>
           <t>LV2 LX2 LC2 LD2</t>
         </is>
       </c>
-      <c r="B79" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C79" s="8" t="inlineStr">
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C80" s="8" t="inlineStr">
         <is>
           <t>http://faderfox.de/lv2.html</t>
         </is>
       </c>
-      <c r="D79" s="8" t="inlineStr">
+      <c r="D80" s="8" t="inlineStr">
         <is>
           <t>Historical: ~$300 each | Limited availability</t>
         </is>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="inlineStr">
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>IK Multimedia</t>
         </is>
       </c>
-      <c r="B81" s="3" t="n"/>
-      <c r="C81" s="3" t="n"/>
-      <c r="D81" s="4" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="inlineStr">
+      <c r="B82" s="3" t="n"/>
+      <c r="C82" s="3" t="n"/>
+      <c r="D82" s="4" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B82" s="5" t="inlineStr">
+      <c r="B83" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C82" s="5" t="inlineStr">
+      <c r="C83" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D82" s="5" t="inlineStr">
+      <c r="D83" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="6" t="inlineStr">
+    <row r="84">
+      <c r="A84" s="6" t="inlineStr">
         <is>
           <t>iRig Keys IO (25/49)</t>
         </is>
       </c>
-      <c r="B83" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C83" s="8" t="inlineStr">
+      <c r="B84" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C84" s="8" t="inlineStr">
         <is>
           <t>https://www.ikmultimedia.com/products/irigkeysio/</t>
         </is>
       </c>
-      <c r="D83" s="8" t="inlineStr">
+      <c r="D84" s="8" t="inlineStr">
         <is>
           <t>$229.99-$329.99</t>
         </is>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="inlineStr">
+    <row r="85"/>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
         <is>
           <t>Korg</t>
         </is>
       </c>
-      <c r="B85" s="3" t="n"/>
-      <c r="C85" s="3" t="n"/>
-      <c r="D85" s="4" t="n"/>
-    </row>
-    <row r="86">
-      <c r="A86" s="5" t="inlineStr">
+      <c r="B86" s="3" t="n"/>
+      <c r="C86" s="3" t="n"/>
+      <c r="D86" s="4" t="n"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B86" s="5" t="inlineStr">
+      <c r="B87" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C86" s="5" t="inlineStr">
+      <c r="C87" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D86" s="5" t="inlineStr">
+      <c r="D87" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="6" t="inlineStr">
-        <is>
-          <t>padKONTROL</t>
-        </is>
-      </c>
-      <c r="B87" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C87" s="8" t="inlineStr">
-        <is>
-          <t>https://www.korg.com/us/products/computergear/padkontrol/</t>
-        </is>
-      </c>
-      <c r="D87" s="8" t="inlineStr">
-        <is>
-          <t>MSRP unknown | Limited</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="6" t="inlineStr">
         <is>
-          <t>Keystage (49/61)</t>
-        </is>
-      </c>
-      <c r="B88" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>padKONTROL</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C88" s="8" t="inlineStr">
         <is>
-          <t>https://www.korg.com/us/products/computergear/keystage/</t>
+          <t>https://www.korg.com/us/products/computergear/padkontrol/</t>
         </is>
       </c>
       <c r="D88" s="8" t="inlineStr">
         <is>
-          <t>$599.99-$699.99</t>
+          <t>MSRP unknown | Limited</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="6" t="inlineStr">
         <is>
+          <t>Keystage (49/61)</t>
+        </is>
+      </c>
+      <c r="B89" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C89" s="8" t="inlineStr">
+        <is>
+          <t>https://www.korg.com/us/products/computergear/keystage/</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>$599.99-$699.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="6" t="inlineStr">
+        <is>
           <t>ZERO8</t>
         </is>
       </c>
-      <c r="B89" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C89" s="8" t="inlineStr">
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C90" s="8" t="inlineStr">
         <is>
           <t>https://www.soundonsound.com/reviews/korg-zero8</t>
         </is>
       </c>
-      <c r="D89" s="8" t="inlineStr">
+      <c r="D90" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Obsolete</t>
         </is>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="inlineStr">
+    <row r="91"/>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
         <is>
           <t>M-Audio</t>
         </is>
       </c>
-      <c r="B91" s="3" t="n"/>
-      <c r="C91" s="3" t="n"/>
-      <c r="D91" s="4" t="n"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="5" t="inlineStr">
+      <c r="B92" s="3" t="n"/>
+      <c r="C92" s="3" t="n"/>
+      <c r="D92" s="4" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B92" s="5" t="inlineStr">
+      <c r="B93" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C92" s="5" t="inlineStr">
+      <c r="C93" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D92" s="5" t="inlineStr">
+      <c r="D93" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="6" t="inlineStr">
-        <is>
-          <t>Axiom (Original)</t>
-        </is>
-      </c>
-      <c r="B93" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C93" s="8" t="inlineStr">
-        <is>
-          <t>https://www.m-audio.com/category/legacy-products.html</t>
-        </is>
-      </c>
-      <c r="D93" s="8" t="inlineStr">
-        <is>
-          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="6" t="inlineStr">
         <is>
-          <t>Axiom 25/49/61 Classic</t>
+          <t>Axiom (Original)</t>
         </is>
       </c>
       <c r="B94" s="7" t="inlineStr">
@@ -2214,7 +2224,7 @@
     <row r="95">
       <c r="A95" s="6" t="inlineStr">
         <is>
-          <t>Axiom AIR (25/49/61/Mini32)</t>
+          <t>Axiom 25/49/61 Classic</t>
         </is>
       </c>
       <c r="B95" s="7" t="inlineStr">
@@ -2229,14 +2239,14 @@
       </c>
       <c r="D95" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="6" t="inlineStr">
         <is>
-          <t>Axiom DirectLink</t>
+          <t>Axiom AIR (25/49/61/Mini32)</t>
         </is>
       </c>
       <c r="B96" s="7" t="inlineStr">
@@ -2251,14 +2261,14 @@
       </c>
       <c r="D96" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Discontinued</t>
+          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="6" t="inlineStr">
         <is>
-          <t>AxiomPro</t>
+          <t>Axiom DirectLink</t>
         </is>
       </c>
       <c r="B97" s="7" t="inlineStr">
@@ -2280,29 +2290,29 @@
     <row r="98">
       <c r="A98" s="6" t="inlineStr">
         <is>
-          <t>Code Series (25/49/61)</t>
-        </is>
-      </c>
-      <c r="B98" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>AxiomPro</t>
+        </is>
+      </c>
+      <c r="B98" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C98" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/</t>
+          <t>https://www.m-audio.com/category/legacy-products.html</t>
         </is>
       </c>
       <c r="D98" s="8" t="inlineStr">
         <is>
-          <t>Original MSRP: $299-399 | Current: $125+</t>
+          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="6" t="inlineStr">
         <is>
-          <t>Hammer 88 Pro</t>
+          <t>Code Series (25/49/61)</t>
         </is>
       </c>
       <c r="B99" s="9" t="inlineStr">
@@ -2317,36 +2327,36 @@
       </c>
       <c r="D99" s="8" t="inlineStr">
         <is>
-          <t>Available at retailers</t>
+          <t>Original MSRP: $299-399 | Current: $125+</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="6" t="inlineStr">
         <is>
-          <t>Keystation Pro 88</t>
-        </is>
-      </c>
-      <c r="B100" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Hammer 88 Pro</t>
+        </is>
+      </c>
+      <c r="B100" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C100" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/category/legacy-products.html</t>
+          <t>https://www.m-audio.com/</t>
         </is>
       </c>
       <c r="D100" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Discontinued</t>
+          <t>Available at retailers</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="6" t="inlineStr">
         <is>
-          <t>O2</t>
+          <t>Keystation Pro 88</t>
         </is>
       </c>
       <c r="B101" s="7" t="inlineStr">
@@ -2361,14 +2371,14 @@
       </c>
       <c r="D101" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="6" t="inlineStr">
         <is>
-          <t>Oxygen8 (Original)</t>
+          <t>O2</t>
         </is>
       </c>
       <c r="B102" s="7" t="inlineStr">
@@ -2383,14 +2393,14 @@
       </c>
       <c r="D102" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Discontinued</t>
+          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="6" t="inlineStr">
         <is>
-          <t>Oxygen8 v2</t>
+          <t>Oxygen8 (Original)</t>
         </is>
       </c>
       <c r="B103" s="7" t="inlineStr">
@@ -2405,36 +2415,36 @@
       </c>
       <c r="D103" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="6" t="inlineStr">
         <is>
-          <t>Oxygen 49/61 (5th Gen)</t>
-        </is>
-      </c>
-      <c r="B104" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Oxygen8 v2</t>
+        </is>
+      </c>
+      <c r="B104" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C104" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/</t>
+          <t>https://www.m-audio.com/category/legacy-products.html</t>
         </is>
       </c>
       <c r="D104" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Current: Available</t>
+          <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="6" t="inlineStr">
         <is>
-          <t>Oxygen Pro (25/49/61)</t>
+          <t>Oxygen 49/61 (5th Gen)</t>
         </is>
       </c>
       <c r="B105" s="9" t="inlineStr">
@@ -2449,14 +2459,14 @@
       </c>
       <c r="D105" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Available</t>
+          <t>MSRP varies | Current: Available</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="6" t="inlineStr">
         <is>
-          <t>Oxygen Pro Mini</t>
+          <t>Oxygen Pro (25/49/61)</t>
         </is>
       </c>
       <c r="B106" s="9" t="inlineStr">
@@ -2466,41 +2476,41 @@
       </c>
       <c r="C106" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/keyboard-controllers/oxygen-pro-mini.html</t>
+          <t>https://www.m-audio.com/</t>
         </is>
       </c>
       <c r="D106" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="6" t="inlineStr">
         <is>
-          <t>Oxygen 3rd Gen</t>
-        </is>
-      </c>
-      <c r="B107" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Oxygen Pro Mini</t>
+        </is>
+      </c>
+      <c r="B107" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C107" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/</t>
+          <t>https://www.m-audio.com/keyboard-controllers/oxygen-pro-mini.html</t>
         </is>
       </c>
       <c r="D107" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="6" t="inlineStr">
         <is>
-          <t>Oxygen 4th Gen</t>
+          <t>Oxygen 3rd Gen</t>
         </is>
       </c>
       <c r="B108" s="7" t="inlineStr">
@@ -2522,7 +2532,7 @@
     <row r="109">
       <c r="A109" s="6" t="inlineStr">
         <is>
-          <t>Ozone</t>
+          <t>Oxygen 4th Gen</t>
         </is>
       </c>
       <c r="B109" s="7" t="inlineStr">
@@ -2532,19 +2542,19 @@
       </c>
       <c r="C109" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/category/legacy-products.html</t>
+          <t>https://www.m-audio.com/</t>
         </is>
       </c>
       <c r="D109" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | No longer available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="6" t="inlineStr">
         <is>
-          <t>Ozonic</t>
+          <t>Ozone</t>
         </is>
       </c>
       <c r="B110" s="7" t="inlineStr">
@@ -2559,14 +2569,14 @@
       </c>
       <c r="D110" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Discontinued</t>
+          <t>MSRP unknown | No longer available</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="6" t="inlineStr">
         <is>
-          <t>ProjectMixIO</t>
+          <t>Ozonic</t>
         </is>
       </c>
       <c r="B111" s="7" t="inlineStr">
@@ -2581,14 +2591,14 @@
       </c>
       <c r="D111" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | End of Life</t>
+          <t>MSRP unknown | Discontinued</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="6" t="inlineStr">
         <is>
-          <t>Radium 49/61</t>
+          <t>ProjectMixIO</t>
         </is>
       </c>
       <c r="B112" s="7" t="inlineStr">
@@ -2603,14 +2613,14 @@
       </c>
       <c r="D112" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | No longer available</t>
+          <t>MSRP unknown | End of Life</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="6" t="inlineStr">
         <is>
-          <t>TriggerFinger (Original)</t>
+          <t>Radium 49/61</t>
         </is>
       </c>
       <c r="B113" s="7" t="inlineStr">
@@ -2620,117 +2630,118 @@
       </c>
       <c r="C113" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/</t>
+          <t>https://www.m-audio.com/category/legacy-products.html</t>
         </is>
       </c>
       <c r="D113" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP unknown | No longer available</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="6" t="inlineStr">
         <is>
-          <t>TriggerFinger Pro</t>
-        </is>
-      </c>
-      <c r="B114" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>TriggerFinger (Original)</t>
+        </is>
+      </c>
+      <c r="B114" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C114" s="8" t="inlineStr">
         <is>
-          <t>https://www.m-audio.com/legacy/trigger-finger-pro.html</t>
+          <t>https://www.m-audio.com/</t>
         </is>
       </c>
       <c r="D114" s="8" t="inlineStr">
         <is>
-          <t>Available at retailers</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="6" t="inlineStr">
         <is>
+          <t>TriggerFinger Pro</t>
+        </is>
+      </c>
+      <c r="B115" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C115" s="8" t="inlineStr">
+        <is>
+          <t>https://www.m-audio.com/legacy/trigger-finger-pro.html</t>
+        </is>
+      </c>
+      <c r="D115" s="8" t="inlineStr">
+        <is>
+          <t>Available at retailers</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="6" t="inlineStr">
+        <is>
           <t>UC33e</t>
         </is>
       </c>
-      <c r="B115" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C115" s="8" t="inlineStr">
+      <c r="B116" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C116" s="8" t="inlineStr">
         <is>
           <t>https://www.m-audio.com/</t>
         </is>
       </c>
-      <c r="D115" s="8" t="inlineStr">
+      <c r="D116" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Out of production</t>
         </is>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="inlineStr">
+    <row r="117"/>
+    <row r="118">
+      <c r="A118" s="2" t="inlineStr">
         <is>
           <t>Mackie</t>
         </is>
       </c>
-      <c r="B117" s="3" t="n"/>
-      <c r="C117" s="3" t="n"/>
-      <c r="D117" s="4" t="n"/>
-    </row>
-    <row r="118">
-      <c r="A118" s="5" t="inlineStr">
+      <c r="B118" s="3" t="n"/>
+      <c r="C118" s="3" t="n"/>
+      <c r="D118" s="4" t="n"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B118" s="5" t="inlineStr">
+      <c r="B119" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C118" s="5" t="inlineStr">
+      <c r="C119" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D118" s="5" t="inlineStr">
+      <c r="D119" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="6" t="inlineStr">
-        <is>
-          <t>MackieControl (Original)</t>
-        </is>
-      </c>
-      <c r="B119" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C119" s="8" t="inlineStr">
-        <is>
-          <t>https://mackie.com/</t>
-        </is>
-      </c>
-      <c r="D119" s="8" t="inlineStr">
-        <is>
-          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="6" t="inlineStr">
         <is>
-          <t>MackieControl Classic</t>
+          <t>MackieControl (Original)</t>
         </is>
       </c>
       <c r="B120" s="7" t="inlineStr">
@@ -2752,88 +2763,89 @@
     <row r="121">
       <c r="A121" s="6" t="inlineStr">
         <is>
+          <t>MackieControl Classic</t>
+        </is>
+      </c>
+      <c r="B121" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C121" s="8" t="inlineStr">
+        <is>
+          <t>https://mackie.com/</t>
+        </is>
+      </c>
+      <c r="D121" s="8" t="inlineStr">
+        <is>
+          <t>MSRP unknown | Superseded</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="6" t="inlineStr">
+        <is>
           <t>MackieControlXT</t>
         </is>
       </c>
-      <c r="B121" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C121" s="8" t="inlineStr">
+      <c r="B122" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C122" s="8" t="inlineStr">
         <is>
           <t>https://mackie.com/</t>
         </is>
       </c>
-      <c r="D121" s="8" t="inlineStr">
+      <c r="D122" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" s="2" t="inlineStr">
+    <row r="123"/>
+    <row r="124">
+      <c r="A124" s="2" t="inlineStr">
         <is>
           <t>Native Instruments</t>
         </is>
       </c>
-      <c r="B123" s="3" t="n"/>
-      <c r="C123" s="3" t="n"/>
-      <c r="D123" s="4" t="n"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="5" t="inlineStr">
+      <c r="B124" s="3" t="n"/>
+      <c r="C124" s="3" t="n"/>
+      <c r="D124" s="4" t="n"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B124" s="5" t="inlineStr">
+      <c r="B125" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C124" s="5" t="inlineStr">
+      <c r="C125" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D124" s="5" t="inlineStr">
+      <c r="D125" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="6" t="inlineStr">
-        <is>
-          <t>Komplete Kontrol A (25/49/61)</t>
-        </is>
-      </c>
-      <c r="B125" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C125" s="8" t="inlineStr">
-        <is>
-          <t>https://www.native-instruments.com/</t>
-        </is>
-      </c>
-      <c r="D125" s="8" t="inlineStr">
-        <is>
-          <t>MSRP: from $169</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="6" t="inlineStr">
         <is>
-          <t>Komplete Kontrol S Mk2 (49/61/88)</t>
-        </is>
-      </c>
-      <c r="B126" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Komplete Kontrol A (25/49/61)</t>
+        </is>
+      </c>
+      <c r="B126" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C126" s="8" t="inlineStr">
@@ -2843,139 +2855,140 @@
       </c>
       <c r="D126" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Being phased out</t>
+          <t>MSRP: from $169</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="6" t="inlineStr">
         <is>
-          <t>Komplete Kontrol S Mk3 (49/61/88)</t>
-        </is>
-      </c>
-      <c r="B127" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Komplete Kontrol S Mk2 (49/61/88)</t>
+        </is>
+      </c>
+      <c r="B127" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C127" s="8" t="inlineStr">
         <is>
-          <t>https://www.native-instruments.com/en/products/komplete/keyboards/kontrol-s49-s61-s88/</t>
+          <t>https://www.native-instruments.com/</t>
         </is>
       </c>
       <c r="D127" s="8" t="inlineStr">
         <is>
-          <t>S88: $1,299 | 2025 release</t>
+          <t>MSRP varies | Being phased out</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="6" t="inlineStr">
         <is>
-          <t>KONTROL49</t>
-        </is>
-      </c>
-      <c r="B128" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Komplete Kontrol S Mk3 (49/61/88)</t>
+        </is>
+      </c>
+      <c r="B128" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C128" s="8" t="inlineStr">
         <is>
-          <t>https://www.native-instruments.com/</t>
+          <t>https://www.native-instruments.com/en/products/komplete/keyboards/kontrol-s49-s61-s88/</t>
         </is>
       </c>
       <c r="D128" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>S88: $1,299 | 2025 release</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="6" t="inlineStr">
         <is>
+          <t>KONTROL49</t>
+        </is>
+      </c>
+      <c r="B129" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C129" s="8" t="inlineStr">
+        <is>
+          <t>https://www.native-instruments.com/</t>
+        </is>
+      </c>
+      <c r="D129" s="8" t="inlineStr">
+        <is>
+          <t>MSRP unknown | Legacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="6" t="inlineStr">
+        <is>
           <t>microKONTROL</t>
         </is>
       </c>
-      <c r="B129" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C129" s="8" t="inlineStr">
+      <c r="B130" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C130" s="8" t="inlineStr">
         <is>
           <t>https://www.native-instruments.com/</t>
         </is>
       </c>
-      <c r="D129" s="8" t="inlineStr">
+      <c r="D130" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Legacy</t>
         </is>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" s="2" t="inlineStr">
+    <row r="131"/>
+    <row r="132">
+      <c r="A132" s="2" t="inlineStr">
         <is>
           <t>Novation</t>
         </is>
       </c>
-      <c r="B131" s="3" t="n"/>
-      <c r="C131" s="3" t="n"/>
-      <c r="D131" s="4" t="n"/>
-    </row>
-    <row r="132">
-      <c r="A132" s="5" t="inlineStr">
+      <c r="B132" s="3" t="n"/>
+      <c r="C132" s="3" t="n"/>
+      <c r="D132" s="4" t="n"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B132" s="5" t="inlineStr">
+      <c r="B133" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C132" s="5" t="inlineStr">
+      <c r="C133" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D132" s="5" t="inlineStr">
+      <c r="D133" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="6" t="inlineStr">
-        <is>
-          <t>Impulse (25/49/61)</t>
-        </is>
-      </c>
-      <c r="B133" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C133" s="8" t="inlineStr">
-        <is>
-          <t>https://novationmusic.com/</t>
-        </is>
-      </c>
-      <c r="D133" s="8" t="inlineStr">
-        <is>
-          <t>Varies | $165-200+ used</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="6" t="inlineStr">
         <is>
-          <t>Launch Control (Original)</t>
-        </is>
-      </c>
-      <c r="B134" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Impulse (25/49/61)</t>
+        </is>
+      </c>
+      <c r="B134" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C134" s="8" t="inlineStr">
@@ -2985,14 +2998,14 @@
       </c>
       <c r="D134" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | ~$83+ if available</t>
+          <t>Varies | $165-200+ used</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="6" t="inlineStr">
         <is>
-          <t>Launch Control XL (MK1)</t>
+          <t>Launch Control (Original)</t>
         </is>
       </c>
       <c r="B135" s="7" t="inlineStr">
@@ -3007,36 +3020,36 @@
       </c>
       <c r="D135" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP unknown | ~$83+ if available</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="6" t="inlineStr">
         <is>
-          <t>Launch Control XL (MK2)</t>
-        </is>
-      </c>
-      <c r="B136" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Launch Control XL (MK1)</t>
+        </is>
+      </c>
+      <c r="B136" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C136" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/products/launch-control-xl-mk2</t>
+          <t>https://novationmusic.com/</t>
         </is>
       </c>
       <c r="D136" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="6" t="inlineStr">
         <is>
-          <t>Launch Control XL 3 (MK3)</t>
+          <t>Launch Control XL (MK2)</t>
         </is>
       </c>
       <c r="B137" s="9" t="inlineStr">
@@ -3046,41 +3059,41 @@
       </c>
       <c r="C137" s="8" t="inlineStr">
         <is>
-          <t>https://us.novationmusic.com/products/launch-control-xl</t>
+          <t>https://novationmusic.com/products/launch-control-xl-mk2</t>
         </is>
       </c>
       <c r="D137" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $249.99 USD</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="6" t="inlineStr">
         <is>
-          <t>Launchkey (Original MK1)</t>
-        </is>
-      </c>
-      <c r="B138" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Launch Control XL 3 (MK3)</t>
+        </is>
+      </c>
+      <c r="B138" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C138" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/</t>
+          <t>https://us.novationmusic.com/products/launch-control-xl</t>
         </is>
       </c>
       <c r="D138" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>MSRP: $249.99 USD</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="6" t="inlineStr">
         <is>
-          <t>Launchkey Mini (Original)</t>
+          <t>Launchkey (Original MK1)</t>
         </is>
       </c>
       <c r="B139" s="7" t="inlineStr">
@@ -3102,29 +3115,29 @@
     <row r="140">
       <c r="A140" s="6" t="inlineStr">
         <is>
-          <t>Launchkey Mini MK3</t>
-        </is>
-      </c>
-      <c r="B140" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Launchkey Mini (Original)</t>
+        </is>
+      </c>
+      <c r="B140" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C140" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/products/launchkey-mini-mk3</t>
+          <t>https://novationmusic.com/</t>
         </is>
       </c>
       <c r="D140" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="6" t="inlineStr">
         <is>
-          <t>Launchkey Mini MK4 (25/37)</t>
+          <t>Launchkey Mini MK3</t>
         </is>
       </c>
       <c r="B141" s="9" t="inlineStr">
@@ -3134,46 +3147,46 @@
       </c>
       <c r="C141" s="8" t="inlineStr">
         <is>
-          <t>https://us.novationmusic.com/products/launchkey-mini-25</t>
+          <t>https://novationmusic.com/products/launchkey-mini-mk3</t>
         </is>
       </c>
       <c r="D141" s="8" t="inlineStr">
         <is>
-          <t>Available - 2025</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="6" t="inlineStr">
         <is>
-          <t>Launchkey MK2</t>
-        </is>
-      </c>
-      <c r="B142" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Launchkey Mini MK4 (25/37)</t>
+        </is>
+      </c>
+      <c r="B142" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C142" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/</t>
+          <t>https://us.novationmusic.com/products/launchkey-mini-25</t>
         </is>
       </c>
       <c r="D142" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>Available - 2025</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="6" t="inlineStr">
         <is>
-          <t>Launchkey MK3 (25/37/49/61)</t>
-        </is>
-      </c>
-      <c r="B143" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Launchkey MK2</t>
+        </is>
+      </c>
+      <c r="B143" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C143" s="8" t="inlineStr">
@@ -3183,14 +3196,14 @@
       </c>
       <c r="D143" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="6" t="inlineStr">
         <is>
-          <t>Launchkey MK4 (25/37/49/61)</t>
+          <t>Launchkey MK3 (25/37/49/61)</t>
         </is>
       </c>
       <c r="B144" s="9" t="inlineStr">
@@ -3200,63 +3213,63 @@
       </c>
       <c r="C144" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/launchkey</t>
+          <t>https://novationmusic.com/</t>
         </is>
       </c>
       <c r="D144" s="8" t="inlineStr">
         <is>
-          <t>$329.99+ | 2025 release</t>
+          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="6" t="inlineStr">
         <is>
-          <t>Launchpad (Original)</t>
-        </is>
-      </c>
-      <c r="B145" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Launchkey MK4 (25/37/49/61)</t>
+        </is>
+      </c>
+      <c r="B145" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C145" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/</t>
+          <t>https://novationmusic.com/launchkey</t>
         </is>
       </c>
       <c r="D145" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>$329.99+ | 2025 release</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="6" t="inlineStr">
         <is>
-          <t>Launchpad Mini MK3</t>
-        </is>
-      </c>
-      <c r="B146" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Launchpad (Original)</t>
+        </is>
+      </c>
+      <c r="B146" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C146" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/products/launchpad-mini-mk3</t>
+          <t>https://novationmusic.com/</t>
         </is>
       </c>
       <c r="D146" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="6" t="inlineStr">
         <is>
-          <t>Launchpad MK2</t>
+          <t>Launchpad Mini MK3</t>
         </is>
       </c>
       <c r="B147" s="9" t="inlineStr">
@@ -3266,24 +3279,24 @@
       </c>
       <c r="C147" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/</t>
+          <t>https://novationmusic.com/products/launchpad-mini-mk3</t>
         </is>
       </c>
       <c r="D147" s="8" t="inlineStr">
         <is>
-          <t>$149.95+</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="6" t="inlineStr">
         <is>
-          <t>Launchpad Pro (Original)</t>
-        </is>
-      </c>
-      <c r="B148" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Launchpad MK2</t>
+        </is>
+      </c>
+      <c r="B148" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C148" s="8" t="inlineStr">
@@ -3293,36 +3306,36 @@
       </c>
       <c r="D148" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Superseded</t>
+          <t>$149.95+</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="6" t="inlineStr">
         <is>
-          <t>Launchpad Pro MK3</t>
-        </is>
-      </c>
-      <c r="B149" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
+          <t>Launchpad Pro (Original)</t>
+        </is>
+      </c>
+      <c r="B149" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
         </is>
       </c>
       <c r="C149" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/products/launchpad-pro-mk3</t>
+          <t>https://novationmusic.com/</t>
         </is>
       </c>
       <c r="D149" s="8" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>MSRP unknown | Superseded</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="6" t="inlineStr">
         <is>
-          <t>Launchpad X</t>
+          <t>Launchpad Pro MK3</t>
         </is>
       </c>
       <c r="B150" s="9" t="inlineStr">
@@ -3332,7 +3345,7 @@
       </c>
       <c r="C150" s="8" t="inlineStr">
         <is>
-          <t>https://novationmusic.com/</t>
+          <t>https://novationmusic.com/products/launchpad-pro-mk3</t>
         </is>
       </c>
       <c r="D150" s="8" t="inlineStr">
@@ -3344,12 +3357,12 @@
     <row r="151">
       <c r="A151" s="6" t="inlineStr">
         <is>
-          <t>RemoteSL / RemoteSL Classic</t>
-        </is>
-      </c>
-      <c r="B151" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>Launchpad X</t>
+        </is>
+      </c>
+      <c r="B151" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C151" s="8" t="inlineStr">
@@ -3359,90 +3372,91 @@
       </c>
       <c r="D151" s="8" t="inlineStr">
         <is>
-          <t>MSRP unknown | Legacy</t>
+          <t>Available</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="6" t="inlineStr">
         <is>
+          <t>RemoteSL / RemoteSL Classic</t>
+        </is>
+      </c>
+      <c r="B152" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C152" s="8" t="inlineStr">
+        <is>
+          <t>https://novationmusic.com/</t>
+        </is>
+      </c>
+      <c r="D152" s="8" t="inlineStr">
+        <is>
+          <t>MSRP unknown | Legacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="6" t="inlineStr">
+        <is>
           <t>SL MkIII (49/61)</t>
         </is>
       </c>
-      <c r="B152" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C152" s="8" t="inlineStr">
+      <c r="B153" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C153" s="8" t="inlineStr">
         <is>
           <t>https://novationmusic.com/en/keys/sl-mkiii</t>
         </is>
       </c>
-      <c r="D152" s="8" t="inlineStr">
+      <c r="D153" s="8" t="inlineStr">
         <is>
           <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
-    <row r="154">
-      <c r="A154" s="2" t="inlineStr">
+    <row r="154"/>
+    <row r="155">
+      <c r="A155" s="2" t="inlineStr">
         <is>
           <t>PreSonus</t>
         </is>
       </c>
-      <c r="B154" s="3" t="n"/>
-      <c r="C154" s="3" t="n"/>
-      <c r="D154" s="4" t="n"/>
-    </row>
-    <row r="155">
-      <c r="A155" s="5" t="inlineStr">
+      <c r="B155" s="3" t="n"/>
+      <c r="C155" s="3" t="n"/>
+      <c r="D155" s="4" t="n"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B155" s="5" t="inlineStr">
+      <c r="B156" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C155" s="5" t="inlineStr">
+      <c r="C156" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D155" s="5" t="inlineStr">
+      <c r="D156" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="6" t="inlineStr">
-        <is>
-          <t>ATOM</t>
-        </is>
-      </c>
-      <c r="B156" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C156" s="8" t="inlineStr">
-        <is>
-          <t>https://www.presonus.com/</t>
-        </is>
-      </c>
-      <c r="D156" s="8" t="inlineStr">
-        <is>
-          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="6" t="inlineStr">
         <is>
-          <t>ATOMSQ</t>
+          <t>ATOM</t>
         </is>
       </c>
       <c r="B157" s="9" t="inlineStr">
@@ -3452,19 +3466,19 @@
       </c>
       <c r="C157" s="8" t="inlineStr">
         <is>
-          <t>https://www.presonus.com/products/ATOM-SQ</t>
+          <t>https://www.presonus.com/</t>
         </is>
       </c>
       <c r="D157" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $250</t>
+          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="6" t="inlineStr">
         <is>
-          <t>FaderPort (Original)</t>
+          <t>ATOMSQ</t>
         </is>
       </c>
       <c r="B158" s="9" t="inlineStr">
@@ -3474,19 +3488,19 @@
       </c>
       <c r="C158" s="8" t="inlineStr">
         <is>
-          <t>https://www.presonus.com/products/faderport</t>
+          <t>https://www.presonus.com/products/ATOM-SQ</t>
         </is>
       </c>
       <c r="D158" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Available</t>
+          <t>MSRP: $250</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="6" t="inlineStr">
         <is>
-          <t>FaderPort 8</t>
+          <t>FaderPort (Original)</t>
         </is>
       </c>
       <c r="B159" s="9" t="inlineStr">
@@ -3496,19 +3510,19 @@
       </c>
       <c r="C159" s="8" t="inlineStr">
         <is>
-          <t>https://www.presonus.com/</t>
+          <t>https://www.presonus.com/products/faderport</t>
         </is>
       </c>
       <c r="D159" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $524.99</t>
+          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="6" t="inlineStr">
         <is>
-          <t>FaderPort 16</t>
+          <t>FaderPort 8</t>
         </is>
       </c>
       <c r="B160" s="9" t="inlineStr">
@@ -3523,220 +3537,223 @@
       </c>
       <c r="D160" s="8" t="inlineStr">
         <is>
-          <t>MSRP: $787.99</t>
+          <t>MSRP: $524.99</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="6" t="inlineStr">
         <is>
+          <t>FaderPort 16</t>
+        </is>
+      </c>
+      <c r="B161" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C161" s="8" t="inlineStr">
+        <is>
+          <t>https://www.presonus.com/</t>
+        </is>
+      </c>
+      <c r="D161" s="8" t="inlineStr">
+        <is>
+          <t>MSRP: $787.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="6" t="inlineStr">
+        <is>
           <t>FaderPort 16 XT</t>
         </is>
       </c>
-      <c r="B161" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C161" s="8" t="inlineStr">
+      <c r="B162" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C162" s="8" t="inlineStr">
         <is>
           <t>https://www.presonus.com/</t>
         </is>
       </c>
-      <c r="D161" s="8" t="inlineStr">
+      <c r="D162" s="8" t="inlineStr">
         <is>
           <t>Status unclear - may not exist</t>
         </is>
       </c>
     </row>
-    <row r="163">
-      <c r="A163" s="2" t="inlineStr">
+    <row r="163"/>
+    <row r="164">
+      <c r="A164" s="2" t="inlineStr">
         <is>
           <t>Reloop</t>
         </is>
       </c>
-      <c r="B163" s="3" t="n"/>
-      <c r="C163" s="3" t="n"/>
-      <c r="D163" s="4" t="n"/>
-    </row>
-    <row r="164">
-      <c r="A164" s="5" t="inlineStr">
+      <c r="B164" s="3" t="n"/>
+      <c r="C164" s="3" t="n"/>
+      <c r="D164" s="4" t="n"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B164" s="5" t="inlineStr">
+      <c r="B165" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C164" s="5" t="inlineStr">
+      <c r="C165" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D164" s="5" t="inlineStr">
+      <c r="D165" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="6" t="inlineStr">
-        <is>
-          <t>KeyFadr</t>
-        </is>
-      </c>
-      <c r="B165" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C165" s="8" t="inlineStr">
-        <is>
-          <t>https://www.reloop.com/reloop-keyfadr</t>
-        </is>
-      </c>
-      <c r="D165" s="8" t="inlineStr">
-        <is>
-          <t>MSRP: $299 | Street: $229</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="6" t="inlineStr">
         <is>
+          <t>KeyFadr</t>
+        </is>
+      </c>
+      <c r="B166" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C166" s="8" t="inlineStr">
+        <is>
+          <t>https://www.reloop.com/reloop-keyfadr</t>
+        </is>
+      </c>
+      <c r="D166" s="8" t="inlineStr">
+        <is>
+          <t>MSRP: $299 | Street: $229</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="6" t="inlineStr">
+        <is>
           <t>KeyPad</t>
         </is>
       </c>
-      <c r="B166" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C166" s="8" t="inlineStr">
+      <c r="B167" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C167" s="8" t="inlineStr">
         <is>
           <t>https://www.reloop.com/reloop-keypad</t>
         </is>
       </c>
-      <c r="D166" s="8" t="inlineStr">
+      <c r="D167" s="8" t="inlineStr">
         <is>
           <t>MSRP unknown | Replaced by KeyPad Pro</t>
         </is>
       </c>
     </row>
-    <row r="168">
-      <c r="A168" s="2" t="inlineStr">
+    <row r="168"/>
+    <row r="169">
+      <c r="A169" s="2" t="inlineStr">
         <is>
           <t>ROLI</t>
         </is>
       </c>
-      <c r="B168" s="3" t="n"/>
-      <c r="C168" s="3" t="n"/>
-      <c r="D168" s="4" t="n"/>
-    </row>
-    <row r="169">
-      <c r="A169" s="5" t="inlineStr">
+      <c r="B169" s="3" t="n"/>
+      <c r="C169" s="3" t="n"/>
+      <c r="D169" s="4" t="n"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B169" s="5" t="inlineStr">
+      <c r="B170" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C169" s="5" t="inlineStr">
+      <c r="C170" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D169" s="5" t="inlineStr">
+      <c r="D170" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
         </is>
       </c>
     </row>
-    <row r="170">
-      <c r="A170" s="6" t="inlineStr">
+    <row r="171">
+      <c r="A171" s="6" t="inlineStr">
         <is>
           <t>BLOCKS</t>
         </is>
       </c>
-      <c r="B170" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C170" s="8" t="inlineStr">
+      <c r="B171" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C171" s="8" t="inlineStr">
         <is>
           <t>https://roli.com/</t>
         </is>
       </c>
-      <c r="D170" s="8" t="inlineStr">
+      <c r="D171" s="8" t="inlineStr">
         <is>
           <t>MSRP varies | Supported</t>
         </is>
       </c>
     </row>
-    <row r="172">
-      <c r="A172" s="2" t="inlineStr">
+    <row r="172"/>
+    <row r="173">
+      <c r="A173" s="2" t="inlineStr">
         <is>
           <t>Roland</t>
         </is>
       </c>
-      <c r="B172" s="3" t="n"/>
-      <c r="C172" s="3" t="n"/>
-      <c r="D172" s="4" t="n"/>
-    </row>
-    <row r="173">
-      <c r="A173" s="5" t="inlineStr">
+      <c r="B173" s="3" t="n"/>
+      <c r="C173" s="3" t="n"/>
+      <c r="D173" s="4" t="n"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B173" s="5" t="inlineStr">
+      <c r="B174" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C173" s="5" t="inlineStr">
+      <c r="C174" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D173" s="5" t="inlineStr">
+      <c r="D174" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="6" t="inlineStr">
-        <is>
-          <t>AIRA MX-1</t>
-        </is>
-      </c>
-      <c r="B174" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C174" s="8" t="inlineStr">
-        <is>
-          <t>https://www.roland.com/</t>
-        </is>
-      </c>
-      <c r="D174" s="8" t="inlineStr">
-        <is>
-          <t>MSRP: $1,279.99 | Current: $381+</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="6" t="inlineStr">
         <is>
-          <t>FANTOM (6/7/8)</t>
+          <t>AIRA MX-1</t>
         </is>
       </c>
       <c r="B175" s="9" t="inlineStr">
@@ -3746,108 +3763,131 @@
       </c>
       <c r="C175" s="8" t="inlineStr">
         <is>
-          <t>https://www.roland.com/global/products/fantom/</t>
+          <t>https://www.roland.com/</t>
         </is>
       </c>
       <c r="D175" s="8" t="inlineStr">
         <is>
-          <t>MSRP varies | Available</t>
+          <t>MSRP: $1,279.99 | Current: $381+</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="6" t="inlineStr">
         <is>
-          <t>A-PRO</t>
-        </is>
-      </c>
-      <c r="B176" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
+          <t>FANTOM (6/7/8)</t>
+        </is>
+      </c>
+      <c r="B176" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
         </is>
       </c>
       <c r="C176" s="8" t="inlineStr">
         <is>
-          <t>https://www.roland.com/</t>
+          <t>https://www.roland.com/global/products/fantom/</t>
         </is>
       </c>
       <c r="D176" s="8" t="inlineStr">
         <is>
-          <t>Status unclear - existence not confirmed</t>
+          <t>MSRP varies | Available</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="6" t="inlineStr">
         <is>
+          <t>A-PRO</t>
+        </is>
+      </c>
+      <c r="B177" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C177" s="8" t="inlineStr">
+        <is>
+          <t>https://www.roland.com/</t>
+        </is>
+      </c>
+      <c r="D177" s="8" t="inlineStr">
+        <is>
+          <t>Status unclear - existence not confirmed</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="6" t="inlineStr">
+        <is>
           <t>FA (FA-06/FA-08)</t>
         </is>
       </c>
-      <c r="B177" s="9" t="inlineStr">
-        <is>
-          <t>Verified</t>
-        </is>
-      </c>
-      <c r="C177" s="8" t="inlineStr">
+      <c r="B178" s="9" t="inlineStr">
+        <is>
+          <t>Verified</t>
+        </is>
+      </c>
+      <c r="C178" s="8" t="inlineStr">
         <is>
           <t>https://www.roland.com/</t>
         </is>
       </c>
-      <c r="D177" s="8" t="inlineStr">
+      <c r="D178" s="8" t="inlineStr">
         <is>
           <t>FA-06 from $800 | Available</t>
         </is>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" s="2" t="inlineStr">
+    <row r="179"/>
+    <row r="180">
+      <c r="A180" s="2" t="inlineStr">
         <is>
           <t>Tascam</t>
         </is>
       </c>
-      <c r="B179" s="3" t="n"/>
-      <c r="C179" s="3" t="n"/>
-      <c r="D179" s="4" t="n"/>
-    </row>
-    <row r="180">
-      <c r="A180" s="5" t="inlineStr">
+      <c r="B180" s="3" t="n"/>
+      <c r="C180" s="3" t="n"/>
+      <c r="D180" s="4" t="n"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="5" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B180" s="5" t="inlineStr">
+      <c r="B181" s="5" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C180" s="5" t="inlineStr">
+      <c r="C181" s="5" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
-      <c r="D180" s="5" t="inlineStr">
+      <c r="D181" s="5" t="inlineStr">
         <is>
           <t>Pricing</t>
         </is>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" s="6" t="inlineStr">
+    <row r="182">
+      <c r="A182" s="6" t="inlineStr">
         <is>
           <t>FireOne</t>
         </is>
       </c>
-      <c r="B181" s="7" t="inlineStr">
-        <is>
-          <t>Discontinued</t>
-        </is>
-      </c>
-      <c r="C181" s="8" t="inlineStr">
+      <c r="B182" s="7" t="inlineStr">
+        <is>
+          <t>Discontinued</t>
+        </is>
+      </c>
+      <c r="C182" s="8" t="inlineStr">
         <is>
           <t>https://tascam.com/us/product/fireone</t>
         </is>
       </c>
-      <c r="D181" s="8" t="inlineStr">
+      <c r="D182" s="8" t="inlineStr">
         <is>
           <t>£209 (~$260 USD) | 2007 release</t>
         </is>

</xml_diff>